<commit_message>
Add my personal daily scrum.
</commit_message>
<xml_diff>
--- a/Dailyscrum_cartwright.xlsx
+++ b/Dailyscrum_cartwright.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\工具\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LZY\Agile and Test-Driven\COMP62521\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" tabRatio="500" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Christos Panagi" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -126,13 +126,49 @@
   </si>
   <si>
     <t>submit the task</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>followed the instructions on blackboard to clone, run and test the code</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>get more familiar with the souce code</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>get full understand of the tasks in sprint1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>finished the test for the calculate_first_last function</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>went through the source code</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>analysed the requirements</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>discussed the sprint1 with team menbers and got the divided work</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed the existed errors and passed the tests</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>finish the test for the new function: calculate_first_last</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3">
     <font>
       <sz val="12"/>
@@ -488,7 +524,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -728,7 +764,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -931,7 +967,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1134,10 +1170,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1377,14 +1413,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="57.4609375" customWidth="1"/>
+    <col min="2" max="2" width="43.84375" customWidth="1"/>
+    <col min="3" max="3" width="41.23046875" customWidth="1"/>
+    <col min="4" max="4" width="42.3046875" customWidth="1"/>
+    <col min="5" max="5" width="23.4609375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
@@ -1450,25 +1493,42 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1477,7 +1537,9 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1524,17 +1586,27 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1542,8 +1614,12 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1551,7 +1627,9 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>

</xml_diff>